<commit_message>
finish my work temporarily
</commit_message>
<xml_diff>
--- a/工作分配.xlsx
+++ b/工作分配.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>郑兴瑞</t>
   </si>
@@ -46,6 +46,12 @@
     <t>李志洋</t>
   </si>
   <si>
+    <t>管理员的借阅记录分析</t>
+  </si>
+  <si>
+    <t>管理员的系统维护</t>
+  </si>
+  <si>
     <t>冯隆腾</t>
   </si>
   <si>
@@ -55,10 +61,10 @@
     <t>图书归还</t>
   </si>
   <si>
-    <t>借阅记录分析*2</t>
-  </si>
-  <si>
-    <t>系统维护*2</t>
+    <t>读者的借阅记录分析</t>
+  </si>
+  <si>
+    <t>读者的系统维护</t>
   </si>
   <si>
     <t>张哲凯</t>
@@ -1004,7 +1010,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -1029,40 +1035,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>